<commit_message>
Added Id to person
</commit_message>
<xml_diff>
--- a/EmailConfirmationServer/Files/TestSheet.xlsx
+++ b/EmailConfirmationServer/Files/TestSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachary.michaels\Source\Repos\emailConfirmationAssistant2\EmailConfirmationServer\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C58D7-8AEB-4B86-9D8B-DD2ECABB306C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B699785B-0C46-457F-B5D5-4175A24E821D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -96,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,15 +462,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -477,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -491,7 +498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -505,17 +512,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added list of emails to person
</commit_message>
<xml_diff>
--- a/EmailConfirmationServer/Files/TestSheet.xlsx
+++ b/EmailConfirmationServer/Files/TestSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachary.michaels\Source\Repos\emailConfirmationAssistant2\EmailConfirmationServer\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B699785B-0C46-457F-B5D5-4175A24E821D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -96,18 +96,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90EE90"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,11 +117,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,7 +452,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,10 +512,10 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed email confirm action
</commit_message>
<xml_diff>
--- a/EmailConfirmationServer/Files/TestSheet.xlsx
+++ b/EmailConfirmationServer/Files/TestSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachary.michaels\Source\Repos\emailConfirmationAssistant2\EmailConfirmationServer\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9833CD-C3CD-4F14-98E6-2B72EFBCC718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -96,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -515,7 +522,7 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added files from project
</commit_message>
<xml_diff>
--- a/EmailConfirmationServer/Files/TestSheet.xlsx
+++ b/EmailConfirmationServer/Files/TestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izmac\Source\Repos\emailConfirmationAssistant-1\EmailConfirmationServer\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456760F1-9624-4FB1-BDAF-17B22C2E392A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -96,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -484,7 +491,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>